<commit_message>
updated design validation plan and schedule
</commit_message>
<xml_diff>
--- a/Project Management/GANTT_Schedule (version 1).xlsx
+++ b/Project Management/GANTT_Schedule (version 1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Molly Meadows\OneDrive - University of Idaho\Documents\2023-2024\Capstone Project\26-Physical-Rehabilitation\Project Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{5E3F26E1-0547-4543-8978-0057A5358D4F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A4D86D-E946-4C38-95E3-0EC2E5FED695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,6 @@
     <sheet name="Schedule" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -37,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="56" uniqueCount="55">
   <si>
     <t>Last Updated:</t>
   </si>
@@ -146,12 +145,6 @@
     <t>Extract Skeletal Data from Smart phone</t>
   </si>
   <si>
-    <t>Compare Skeletal data in training model</t>
-  </si>
-  <si>
-    <t>Build Training model</t>
-  </si>
-  <si>
     <t>Ensure Accuracy of training model</t>
   </si>
   <si>
@@ -203,9 +196,6 @@
     <t>Apr. 26</t>
   </si>
   <si>
-    <t>Collect a database of videos for analysis</t>
-  </si>
-  <si>
     <t>IF TIME</t>
   </si>
   <si>
@@ -216,6 +206,21 @@
   </si>
   <si>
     <t>Red = Behind Schedule</t>
+  </si>
+  <si>
+    <t>Read and Understand Project Background and Research Papers</t>
+  </si>
+  <si>
+    <t>Data Preprocessing</t>
+  </si>
+  <si>
+    <t>Convert Motions into tokens uping MotionGPT</t>
+  </si>
+  <si>
+    <t>Process Movements using MotionGPT and generate feedback</t>
+  </si>
+  <si>
+    <t>Collect a database of videos for analysis and repeat procedure</t>
   </si>
 </sst>
 </file>
@@ -280,7 +285,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -319,7 +324,13 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.59999389629810485"/>
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -384,7 +395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="35">
+  <cellXfs count="37">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -443,10 +454,7 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="16" fontId="2" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="6" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -468,6 +476,11 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -497,7 +510,7 @@
     <xdr:to>
       <xdr:col>4</xdr:col>
       <xdr:colOff>85725</xdr:colOff>
-      <xdr:row>28</xdr:row>
+      <xdr:row>30</xdr:row>
       <xdr:rowOff>161925</xdr:rowOff>
     </xdr:to>
     <xdr:cxnSp macro="">
@@ -806,13 +819,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:BD37"/>
+  <dimension ref="A1:BD39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="G13" sqref="G13"/>
+      <selection pane="bottomRight" activeCell="D32" sqref="D32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -840,12 +853,12 @@
       <c r="D3" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="30">
+      <c r="E3" s="27">
         <v>45199</v>
       </c>
-      <c r="F3" s="30"/>
-      <c r="H3" s="29"/>
-      <c r="I3" s="29"/>
+      <c r="F3" s="27"/>
+      <c r="H3" s="26"/>
+      <c r="I3" s="26"/>
     </row>
     <row r="4" spans="1:56" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3"/>
@@ -853,49 +866,49 @@
       <c r="D4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="31">
+      <c r="E4" s="28">
         <v>2023</v>
       </c>
-      <c r="F4" s="32"/>
-      <c r="G4" s="32"/>
-      <c r="H4" s="32"/>
-      <c r="I4" s="32"/>
-      <c r="J4" s="32"/>
-      <c r="K4" s="32"/>
-      <c r="L4" s="32"/>
-      <c r="M4" s="32"/>
-      <c r="N4" s="32"/>
-      <c r="O4" s="32"/>
-      <c r="P4" s="32"/>
-      <c r="Q4" s="32"/>
-      <c r="R4" s="32"/>
-      <c r="S4" s="32"/>
-      <c r="T4" s="32"/>
-      <c r="U4" s="32"/>
-      <c r="V4" s="33">
+      <c r="F4" s="29"/>
+      <c r="G4" s="29"/>
+      <c r="H4" s="29"/>
+      <c r="I4" s="29"/>
+      <c r="J4" s="29"/>
+      <c r="K4" s="29"/>
+      <c r="L4" s="29"/>
+      <c r="M4" s="29"/>
+      <c r="N4" s="29"/>
+      <c r="O4" s="29"/>
+      <c r="P4" s="29"/>
+      <c r="Q4" s="29"/>
+      <c r="R4" s="29"/>
+      <c r="S4" s="29"/>
+      <c r="T4" s="29"/>
+      <c r="U4" s="29"/>
+      <c r="V4" s="30">
         <v>2024</v>
       </c>
-      <c r="W4" s="33"/>
-      <c r="X4" s="33"/>
-      <c r="Y4" s="33"/>
-      <c r="Z4" s="33"/>
-      <c r="AA4" s="33"/>
-      <c r="AB4" s="33"/>
-      <c r="AC4" s="33"/>
-      <c r="AD4" s="33"/>
-      <c r="AE4" s="33"/>
-      <c r="AF4" s="33"/>
-      <c r="AG4" s="33"/>
-      <c r="AH4" s="33"/>
-      <c r="AI4" s="33"/>
-      <c r="AJ4" s="33"/>
-      <c r="AK4" s="33"/>
-      <c r="AL4" s="33"/>
-      <c r="AM4" s="33"/>
-      <c r="AN4" s="33"/>
-      <c r="AO4" s="33"/>
-      <c r="AP4" s="33"/>
-      <c r="AQ4" s="33"/>
+      <c r="W4" s="30"/>
+      <c r="X4" s="30"/>
+      <c r="Y4" s="30"/>
+      <c r="Z4" s="30"/>
+      <c r="AA4" s="30"/>
+      <c r="AB4" s="30"/>
+      <c r="AC4" s="30"/>
+      <c r="AD4" s="30"/>
+      <c r="AE4" s="30"/>
+      <c r="AF4" s="30"/>
+      <c r="AG4" s="30"/>
+      <c r="AH4" s="30"/>
+      <c r="AI4" s="30"/>
+      <c r="AJ4" s="30"/>
+      <c r="AK4" s="30"/>
+      <c r="AL4" s="30"/>
+      <c r="AM4" s="30"/>
+      <c r="AN4" s="30"/>
+      <c r="AO4" s="30"/>
+      <c r="AP4" s="30"/>
+      <c r="AQ4" s="30"/>
     </row>
     <row r="5" spans="1:56" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3"/>
@@ -903,63 +916,63 @@
       <c r="D5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="34" t="s">
+      <c r="E5" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="28"/>
-      <c r="G5" s="28"/>
-      <c r="H5" s="28"/>
-      <c r="I5" s="28" t="s">
+      <c r="F5" s="25"/>
+      <c r="G5" s="25"/>
+      <c r="H5" s="25"/>
+      <c r="I5" s="25" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="28"/>
-      <c r="K5" s="28"/>
-      <c r="L5" s="28"/>
-      <c r="M5" s="28"/>
-      <c r="N5" s="28" t="s">
+      <c r="J5" s="25"/>
+      <c r="K5" s="25"/>
+      <c r="L5" s="25"/>
+      <c r="M5" s="25"/>
+      <c r="N5" s="25" t="s">
         <v>5</v>
       </c>
-      <c r="O5" s="28"/>
-      <c r="P5" s="28"/>
-      <c r="Q5" s="28"/>
-      <c r="R5" s="28" t="s">
+      <c r="O5" s="25"/>
+      <c r="P5" s="25"/>
+      <c r="Q5" s="25"/>
+      <c r="R5" s="25" t="s">
         <v>6</v>
       </c>
-      <c r="S5" s="28"/>
-      <c r="T5" s="28"/>
-      <c r="U5" s="28"/>
-      <c r="V5" s="28" t="s">
+      <c r="S5" s="25"/>
+      <c r="T5" s="25"/>
+      <c r="U5" s="25"/>
+      <c r="V5" s="25" t="s">
         <v>7</v>
       </c>
-      <c r="W5" s="28"/>
-      <c r="X5" s="28"/>
-      <c r="Y5" s="28"/>
-      <c r="Z5" s="28"/>
-      <c r="AA5" s="28" t="s">
+      <c r="W5" s="25"/>
+      <c r="X5" s="25"/>
+      <c r="Y5" s="25"/>
+      <c r="Z5" s="25"/>
+      <c r="AA5" s="25" t="s">
         <v>8</v>
       </c>
-      <c r="AB5" s="28"/>
-      <c r="AC5" s="28"/>
-      <c r="AD5" s="28"/>
-      <c r="AE5" s="28" t="s">
+      <c r="AB5" s="25"/>
+      <c r="AC5" s="25"/>
+      <c r="AD5" s="25"/>
+      <c r="AE5" s="25" t="s">
         <v>9</v>
       </c>
-      <c r="AF5" s="28"/>
-      <c r="AG5" s="28"/>
-      <c r="AH5" s="28"/>
-      <c r="AI5" s="28" t="s">
+      <c r="AF5" s="25"/>
+      <c r="AG5" s="25"/>
+      <c r="AH5" s="25"/>
+      <c r="AI5" s="25" t="s">
         <v>10</v>
       </c>
-      <c r="AJ5" s="28"/>
-      <c r="AK5" s="28"/>
-      <c r="AL5" s="28"/>
-      <c r="AM5" s="28" t="s">
+      <c r="AJ5" s="25"/>
+      <c r="AK5" s="25"/>
+      <c r="AL5" s="25"/>
+      <c r="AM5" s="25" t="s">
         <v>11</v>
       </c>
-      <c r="AN5" s="28"/>
-      <c r="AO5" s="28"/>
-      <c r="AP5" s="28"/>
-      <c r="AQ5" s="28"/>
+      <c r="AN5" s="25"/>
+      <c r="AO5" s="25"/>
+      <c r="AP5" s="25"/>
+      <c r="AQ5" s="25"/>
     </row>
     <row r="6" spans="1:56" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
@@ -967,7 +980,7 @@
         <v>13</v>
       </c>
       <c r="C6" s="19" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="D6" s="19" t="s">
         <v>12</v>
@@ -1264,12 +1277,12 @@
         <v>25</v>
       </c>
       <c r="C9" s="15" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D9" s="17"/>
-      <c r="E9" s="25"/>
-      <c r="F9" s="25"/>
-      <c r="G9" s="25"/>
+      <c r="E9" s="24"/>
+      <c r="F9" s="24"/>
+      <c r="G9" s="24"/>
       <c r="H9" s="16"/>
       <c r="I9" s="16"/>
       <c r="J9" s="16"/>
@@ -1312,14 +1325,14 @@
         <v>16</v>
       </c>
       <c r="C10" s="15" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="D10" s="15"/>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
-      <c r="G10" s="27"/>
-      <c r="H10" s="27"/>
-      <c r="I10" s="27"/>
+      <c r="G10" s="32"/>
+      <c r="H10" s="32"/>
+      <c r="I10" s="32"/>
       <c r="J10" s="14"/>
       <c r="K10" s="14"/>
       <c r="L10" s="14"/>
@@ -1360,15 +1373,15 @@
         <v>17</v>
       </c>
       <c r="C11" s="14" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D11" s="14"/>
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
-      <c r="H11" s="14"/>
-      <c r="I11" s="14"/>
-      <c r="J11" s="14"/>
+      <c r="H11" s="33"/>
+      <c r="I11" s="33"/>
+      <c r="J11" s="33"/>
       <c r="K11" s="14"/>
       <c r="L11" s="14"/>
       <c r="M11" s="14"/>
@@ -1408,7 +1421,7 @@
         <v>18</v>
       </c>
       <c r="C12" s="14" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D12" s="14"/>
       <c r="E12" s="14"/>
@@ -1417,11 +1430,11 @@
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
-      <c r="K12" s="14"/>
-      <c r="L12" s="14"/>
-      <c r="M12" s="14"/>
-      <c r="N12" s="14"/>
-      <c r="O12" s="14"/>
+      <c r="K12" s="34"/>
+      <c r="L12" s="34"/>
+      <c r="M12" s="34"/>
+      <c r="N12" s="34"/>
+      <c r="O12" s="34"/>
       <c r="P12" s="14"/>
       <c r="Q12" s="14"/>
       <c r="R12" s="14"/>
@@ -1456,7 +1469,7 @@
         <v>19</v>
       </c>
       <c r="C13" s="14" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D13" s="14"/>
       <c r="E13" s="14"/>
@@ -1504,7 +1517,7 @@
         <v>20</v>
       </c>
       <c r="C14" s="14" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="D14" s="14"/>
       <c r="E14" s="14"/>
@@ -1552,7 +1565,7 @@
         <v>21</v>
       </c>
       <c r="C15" s="14" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D15" s="14"/>
       <c r="E15" s="14"/>
@@ -1600,7 +1613,7 @@
         <v>22</v>
       </c>
       <c r="C16" s="14" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="D16" s="14"/>
       <c r="E16" s="14"/>
@@ -1648,7 +1661,7 @@
         <v>23</v>
       </c>
       <c r="C17" s="14" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D17" s="14"/>
       <c r="E17" s="14"/>
@@ -1830,19 +1843,19 @@
       <c r="AQ20" s="14"/>
     </row>
     <row r="21" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B21" s="14" t="s">
-        <v>28</v>
+      <c r="B21" s="35" t="s">
+        <v>50</v>
       </c>
       <c r="C21" s="23">
-        <v>45209</v>
+        <v>45200</v>
       </c>
       <c r="D21" s="14"/>
-      <c r="E21" s="14"/>
-      <c r="F21" s="14"/>
-      <c r="G21" s="26"/>
-      <c r="H21" s="26"/>
-      <c r="I21" s="26"/>
-      <c r="J21" s="26"/>
+      <c r="E21" s="33"/>
+      <c r="F21" s="33"/>
+      <c r="G21" s="33"/>
+      <c r="H21" s="33"/>
+      <c r="I21" s="14"/>
+      <c r="J21" s="14"/>
       <c r="K21" s="14"/>
       <c r="L21" s="14"/>
       <c r="M21" s="14"/>
@@ -1879,23 +1892,23 @@
     </row>
     <row r="22" spans="2:43" x14ac:dyDescent="0.3">
       <c r="B22" s="14" t="s">
-        <v>48</v>
+        <v>28</v>
       </c>
       <c r="C22" s="23">
-        <v>45226</v>
+        <v>45209</v>
       </c>
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>
-      <c r="G22" s="14"/>
-      <c r="H22" s="14"/>
-      <c r="I22" s="14"/>
-      <c r="J22" s="14"/>
-      <c r="K22" s="14"/>
-      <c r="L22" s="14"/>
-      <c r="M22" s="14"/>
-      <c r="N22" s="14"/>
-      <c r="O22" s="14"/>
+      <c r="G22" s="34"/>
+      <c r="H22" s="34"/>
+      <c r="I22" s="34"/>
+      <c r="J22" s="34"/>
+      <c r="K22" s="34"/>
+      <c r="L22" s="34"/>
+      <c r="M22" s="34"/>
+      <c r="N22" s="34"/>
+      <c r="O22" s="34"/>
       <c r="P22" s="14"/>
       <c r="Q22" s="14"/>
       <c r="R22" s="14"/>
@@ -1927,7 +1940,7 @@
     </row>
     <row r="23" spans="2:43" x14ac:dyDescent="0.3">
       <c r="B23" s="14" t="s">
-        <v>30</v>
+        <v>51</v>
       </c>
       <c r="C23" s="23">
         <v>45260</v>
@@ -1935,15 +1948,15 @@
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
       <c r="F23" s="14"/>
-      <c r="G23" s="14"/>
-      <c r="H23" s="14"/>
-      <c r="I23" s="14"/>
-      <c r="J23" s="14"/>
-      <c r="K23" s="14"/>
-      <c r="L23" s="14"/>
-      <c r="M23" s="14"/>
-      <c r="N23" s="14"/>
-      <c r="O23" s="14"/>
+      <c r="G23" s="36"/>
+      <c r="H23" s="36"/>
+      <c r="I23" s="36"/>
+      <c r="J23" s="36"/>
+      <c r="K23" s="36"/>
+      <c r="L23" s="36"/>
+      <c r="M23" s="36"/>
+      <c r="N23" s="36"/>
+      <c r="O23" s="36"/>
       <c r="P23" s="14"/>
       <c r="Q23" s="14"/>
       <c r="R23" s="14"/>
@@ -1973,48 +1986,48 @@
       <c r="AP23" s="14"/>
       <c r="AQ23" s="14"/>
     </row>
-    <row r="24" spans="2:43" s="2" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="24" spans="2:43" x14ac:dyDescent="0.3">
       <c r="B24" s="14" t="s">
-        <v>29</v>
-      </c>
-      <c r="C24" s="24">
+        <v>52</v>
+      </c>
+      <c r="C24" s="23">
         <v>45281</v>
       </c>
-      <c r="D24" s="16"/>
-      <c r="E24" s="16"/>
-      <c r="F24" s="16"/>
-      <c r="G24" s="16"/>
-      <c r="H24" s="16"/>
-      <c r="I24" s="16"/>
-      <c r="J24" s="16"/>
-      <c r="K24" s="16"/>
-      <c r="L24" s="16"/>
-      <c r="M24" s="16"/>
-      <c r="N24" s="16"/>
-      <c r="O24" s="16"/>
-      <c r="P24" s="16"/>
-      <c r="Q24" s="16"/>
-      <c r="R24" s="16"/>
-      <c r="S24" s="16"/>
-      <c r="T24" s="16"/>
-      <c r="U24" s="16"/>
-      <c r="V24" s="16"/>
-      <c r="W24" s="16"/>
-      <c r="X24" s="16"/>
-      <c r="Y24" s="16"/>
-      <c r="Z24" s="16"/>
-      <c r="AA24" s="16"/>
-      <c r="AB24" s="16"/>
-      <c r="AC24" s="16"/>
-      <c r="AD24" s="16"/>
-      <c r="AE24" s="16"/>
-      <c r="AF24" s="16"/>
-      <c r="AG24" s="16"/>
-      <c r="AH24" s="16"/>
-      <c r="AI24" s="16"/>
-      <c r="AJ24" s="16"/>
-      <c r="AK24" s="16"/>
-      <c r="AL24" s="16"/>
+      <c r="D24" s="14"/>
+      <c r="E24" s="14"/>
+      <c r="F24" s="14"/>
+      <c r="G24" s="36"/>
+      <c r="H24" s="36"/>
+      <c r="I24" s="36"/>
+      <c r="J24" s="36"/>
+      <c r="K24" s="36"/>
+      <c r="L24" s="36"/>
+      <c r="M24" s="36"/>
+      <c r="N24" s="36"/>
+      <c r="O24" s="36"/>
+      <c r="P24" s="14"/>
+      <c r="Q24" s="14"/>
+      <c r="R24" s="14"/>
+      <c r="S24" s="14"/>
+      <c r="T24" s="14"/>
+      <c r="U24" s="14"/>
+      <c r="V24" s="14"/>
+      <c r="W24" s="14"/>
+      <c r="X24" s="14"/>
+      <c r="Y24" s="14"/>
+      <c r="Z24" s="14"/>
+      <c r="AA24" s="14"/>
+      <c r="AB24" s="14"/>
+      <c r="AC24" s="14"/>
+      <c r="AD24" s="14"/>
+      <c r="AE24" s="14"/>
+      <c r="AF24" s="14"/>
+      <c r="AG24" s="14"/>
+      <c r="AH24" s="14"/>
+      <c r="AI24" s="14"/>
+      <c r="AJ24" s="14"/>
+      <c r="AK24" s="14"/>
+      <c r="AL24" s="14"/>
       <c r="AM24" s="16"/>
       <c r="AN24" s="16"/>
       <c r="AO24" s="14"/>
@@ -2026,7 +2039,7 @@
         <v>31</v>
       </c>
       <c r="C25" s="23">
-        <v>44951</v>
+        <v>44986</v>
       </c>
       <c r="D25" s="14"/>
       <c r="E25" s="14"/>
@@ -2071,7 +2084,7 @@
     </row>
     <row r="26" spans="2:43" x14ac:dyDescent="0.3">
       <c r="B26" s="14" t="s">
-        <v>32</v>
+        <v>53</v>
       </c>
       <c r="C26" s="23">
         <v>44958</v>
@@ -2079,15 +2092,15 @@
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
       <c r="F26" s="14"/>
-      <c r="G26" s="14"/>
-      <c r="H26" s="14"/>
-      <c r="I26" s="14"/>
-      <c r="J26" s="14"/>
-      <c r="K26" s="14"/>
-      <c r="L26" s="14"/>
-      <c r="M26" s="14"/>
-      <c r="N26" s="14"/>
-      <c r="O26" s="14"/>
+      <c r="G26" s="36"/>
+      <c r="H26" s="36"/>
+      <c r="I26" s="36"/>
+      <c r="J26" s="36"/>
+      <c r="K26" s="36"/>
+      <c r="L26" s="36"/>
+      <c r="M26" s="36"/>
+      <c r="N26" s="36"/>
+      <c r="O26" s="36"/>
       <c r="P26" s="14"/>
       <c r="Q26" s="14"/>
       <c r="R26" s="14"/>
@@ -2119,10 +2132,10 @@
     </row>
     <row r="27" spans="2:43" x14ac:dyDescent="0.3">
       <c r="B27" s="14" t="s">
-        <v>33</v>
+        <v>30</v>
       </c>
       <c r="C27" s="23">
-        <v>44986</v>
+        <v>44958</v>
       </c>
       <c r="D27" s="14"/>
       <c r="E27" s="14"/>
@@ -2167,10 +2180,10 @@
     </row>
     <row r="28" spans="2:43" x14ac:dyDescent="0.3">
       <c r="B28" s="14" t="s">
-        <v>34</v>
+        <v>54</v>
       </c>
       <c r="C28" s="23">
-        <v>45017</v>
+        <v>44986</v>
       </c>
       <c r="D28" s="14"/>
       <c r="E28" s="14"/>
@@ -2215,11 +2228,12 @@
     </row>
     <row r="29" spans="2:43" x14ac:dyDescent="0.3">
       <c r="B29" s="14" t="s">
-        <v>35</v>
-      </c>
-      <c r="C29" s="14" t="s">
-        <v>49</v>
-      </c>
+        <v>29</v>
+      </c>
+      <c r="C29" s="23">
+        <v>44986</v>
+      </c>
+      <c r="D29" s="14"/>
       <c r="E29" s="14"/>
       <c r="F29" s="14"/>
       <c r="G29" s="14"/>
@@ -2254,41 +2268,136 @@
       <c r="AJ29" s="14"/>
       <c r="AK29" s="14"/>
       <c r="AL29" s="14"/>
-      <c r="AM29" s="14"/>
-      <c r="AN29" s="14"/>
+      <c r="AM29" s="16"/>
+      <c r="AN29" s="16"/>
       <c r="AO29" s="14"/>
       <c r="AP29" s="14"/>
       <c r="AQ29" s="14"/>
     </row>
     <row r="30" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B30" s="22" t="s">
-        <v>36</v>
-      </c>
-      <c r="C30" t="s">
+      <c r="B30" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="C30" s="23">
+        <v>45017</v>
+      </c>
+      <c r="D30" s="14"/>
+      <c r="E30" s="14"/>
+      <c r="F30" s="14"/>
+      <c r="G30" s="14"/>
+      <c r="H30" s="14"/>
+      <c r="I30" s="14"/>
+      <c r="J30" s="14"/>
+      <c r="K30" s="14"/>
+      <c r="L30" s="14"/>
+      <c r="M30" s="14"/>
+      <c r="N30" s="14"/>
+      <c r="O30" s="14"/>
+      <c r="P30" s="14"/>
+      <c r="Q30" s="14"/>
+      <c r="R30" s="14"/>
+      <c r="S30" s="14"/>
+      <c r="T30" s="14"/>
+      <c r="U30" s="14"/>
+      <c r="V30" s="14"/>
+      <c r="W30" s="14"/>
+      <c r="X30" s="14"/>
+      <c r="Y30" s="14"/>
+      <c r="Z30" s="14"/>
+      <c r="AA30" s="14"/>
+      <c r="AB30" s="14"/>
+      <c r="AC30" s="14"/>
+      <c r="AD30" s="14"/>
+      <c r="AE30" s="14"/>
+      <c r="AF30" s="14"/>
+      <c r="AG30" s="14"/>
+      <c r="AH30" s="14"/>
+      <c r="AI30" s="14"/>
+      <c r="AJ30" s="14"/>
+      <c r="AK30" s="14"/>
+      <c r="AL30" s="14"/>
+      <c r="AM30" s="16"/>
+      <c r="AN30" s="16"/>
+      <c r="AO30" s="14"/>
+      <c r="AP30" s="14"/>
+      <c r="AQ30" s="14"/>
+    </row>
+    <row r="31" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="B31" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C31" s="23">
+        <v>45036</v>
+      </c>
+      <c r="E31" s="14"/>
+      <c r="F31" s="14"/>
+      <c r="G31" s="14"/>
+      <c r="H31" s="14"/>
+      <c r="I31" s="14"/>
+      <c r="J31" s="14"/>
+      <c r="K31" s="14"/>
+      <c r="L31" s="14"/>
+      <c r="M31" s="14"/>
+      <c r="N31" s="14"/>
+      <c r="O31" s="14"/>
+      <c r="P31" s="14"/>
+      <c r="Q31" s="14"/>
+      <c r="R31" s="14"/>
+      <c r="S31" s="14"/>
+      <c r="T31" s="14"/>
+      <c r="U31" s="14"/>
+      <c r="V31" s="14"/>
+      <c r="W31" s="14"/>
+      <c r="X31" s="14"/>
+      <c r="Y31" s="14"/>
+      <c r="Z31" s="14"/>
+      <c r="AA31" s="14"/>
+      <c r="AB31" s="14"/>
+      <c r="AC31" s="14"/>
+      <c r="AD31" s="14"/>
+      <c r="AE31" s="14"/>
+      <c r="AF31" s="14"/>
+      <c r="AG31" s="14"/>
+      <c r="AH31" s="14"/>
+      <c r="AI31" s="14"/>
+      <c r="AJ31" s="14"/>
+      <c r="AK31" s="14"/>
+      <c r="AL31" s="14"/>
+      <c r="AM31" s="14"/>
+      <c r="AN31" s="14"/>
+      <c r="AO31" s="14"/>
+      <c r="AP31" s="14"/>
+      <c r="AQ31" s="14"/>
+    </row>
+    <row r="32" spans="2:43" x14ac:dyDescent="0.3">
+      <c r="B32" s="22" t="s">
+        <v>34</v>
+      </c>
+      <c r="C32" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="33" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B33" s="22" t="s">
+        <v>35</v>
+      </c>
+      <c r="C33" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="37" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B37" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="38" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B38" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="39" spans="2:3" x14ac:dyDescent="0.3">
+      <c r="B39" t="s">
         <v>49</v>
-      </c>
-    </row>
-    <row r="31" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B31" s="22" t="s">
-        <v>37</v>
-      </c>
-      <c r="C31" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B35" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B36" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.3">
-      <c r="B37" t="s">
-        <v>52</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Agenda for meeting for 10-25
</commit_message>
<xml_diff>
--- a/Project Management/GANTT_Schedule (version 1).xlsx
+++ b/Project Management/GANTT_Schedule (version 1).xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Molly Meadows\OneDrive - University of Idaho\Documents\2023-2024\Capstone Project\26-Physical-Rehabilitation\Project Management\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A4D86D-E946-4C38-95E3-0EC2E5FED695}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80514DD3-B476-4778-858E-AEF8DBC8F60B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -395,7 +395,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="37">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -455,6 +455,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="16" fontId="0" fillId="0" borderId="2" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -476,11 +480,6 @@
     <xf numFmtId="0" fontId="2" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="6" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -822,10 +821,10 @@
   <dimension ref="A1:BD39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="6" topLeftCell="C11" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="6" topLeftCell="C7" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A7" sqref="A7"/>
-      <selection pane="bottomRight" activeCell="D32" sqref="D32"/>
+      <selection pane="bottomRight" activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" outlineLevelCol="1" x14ac:dyDescent="0.3"/>
@@ -853,12 +852,12 @@
       <c r="D3" s="20" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="27">
-        <v>45199</v>
-      </c>
-      <c r="F3" s="27"/>
-      <c r="H3" s="26"/>
-      <c r="I3" s="26"/>
+      <c r="E3" s="31">
+        <v>45221</v>
+      </c>
+      <c r="F3" s="31"/>
+      <c r="H3" s="30"/>
+      <c r="I3" s="30"/>
     </row>
     <row r="4" spans="1:56" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B4" s="3"/>
@@ -866,49 +865,49 @@
       <c r="D4" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="E4" s="28">
+      <c r="E4" s="32">
         <v>2023</v>
       </c>
-      <c r="F4" s="29"/>
-      <c r="G4" s="29"/>
-      <c r="H4" s="29"/>
-      <c r="I4" s="29"/>
-      <c r="J4" s="29"/>
-      <c r="K4" s="29"/>
-      <c r="L4" s="29"/>
-      <c r="M4" s="29"/>
-      <c r="N4" s="29"/>
-      <c r="O4" s="29"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="29"/>
-      <c r="R4" s="29"/>
-      <c r="S4" s="29"/>
-      <c r="T4" s="29"/>
-      <c r="U4" s="29"/>
-      <c r="V4" s="30">
+      <c r="F4" s="33"/>
+      <c r="G4" s="33"/>
+      <c r="H4" s="33"/>
+      <c r="I4" s="33"/>
+      <c r="J4" s="33"/>
+      <c r="K4" s="33"/>
+      <c r="L4" s="33"/>
+      <c r="M4" s="33"/>
+      <c r="N4" s="33"/>
+      <c r="O4" s="33"/>
+      <c r="P4" s="33"/>
+      <c r="Q4" s="33"/>
+      <c r="R4" s="33"/>
+      <c r="S4" s="33"/>
+      <c r="T4" s="33"/>
+      <c r="U4" s="33"/>
+      <c r="V4" s="34">
         <v>2024</v>
       </c>
-      <c r="W4" s="30"/>
-      <c r="X4" s="30"/>
-      <c r="Y4" s="30"/>
-      <c r="Z4" s="30"/>
-      <c r="AA4" s="30"/>
-      <c r="AB4" s="30"/>
-      <c r="AC4" s="30"/>
-      <c r="AD4" s="30"/>
-      <c r="AE4" s="30"/>
-      <c r="AF4" s="30"/>
-      <c r="AG4" s="30"/>
-      <c r="AH4" s="30"/>
-      <c r="AI4" s="30"/>
-      <c r="AJ4" s="30"/>
-      <c r="AK4" s="30"/>
-      <c r="AL4" s="30"/>
-      <c r="AM4" s="30"/>
-      <c r="AN4" s="30"/>
-      <c r="AO4" s="30"/>
-      <c r="AP4" s="30"/>
-      <c r="AQ4" s="30"/>
+      <c r="W4" s="34"/>
+      <c r="X4" s="34"/>
+      <c r="Y4" s="34"/>
+      <c r="Z4" s="34"/>
+      <c r="AA4" s="34"/>
+      <c r="AB4" s="34"/>
+      <c r="AC4" s="34"/>
+      <c r="AD4" s="34"/>
+      <c r="AE4" s="34"/>
+      <c r="AF4" s="34"/>
+      <c r="AG4" s="34"/>
+      <c r="AH4" s="34"/>
+      <c r="AI4" s="34"/>
+      <c r="AJ4" s="34"/>
+      <c r="AK4" s="34"/>
+      <c r="AL4" s="34"/>
+      <c r="AM4" s="34"/>
+      <c r="AN4" s="34"/>
+      <c r="AO4" s="34"/>
+      <c r="AP4" s="34"/>
+      <c r="AQ4" s="34"/>
     </row>
     <row r="5" spans="1:56" s="2" customFormat="1" x14ac:dyDescent="0.3">
       <c r="B5" s="3"/>
@@ -916,63 +915,63 @@
       <c r="D5" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E5" s="31" t="s">
+      <c r="E5" s="35" t="s">
         <v>3</v>
       </c>
-      <c r="F5" s="25"/>
-      <c r="G5" s="25"/>
-      <c r="H5" s="25"/>
-      <c r="I5" s="25" t="s">
+      <c r="F5" s="29"/>
+      <c r="G5" s="29"/>
+      <c r="H5" s="29"/>
+      <c r="I5" s="29" t="s">
         <v>4</v>
       </c>
-      <c r="J5" s="25"/>
-      <c r="K5" s="25"/>
-      <c r="L5" s="25"/>
-      <c r="M5" s="25"/>
-      <c r="N5" s="25" t="s">
+      <c r="J5" s="29"/>
+      <c r="K5" s="29"/>
+      <c r="L5" s="29"/>
+      <c r="M5" s="29"/>
+      <c r="N5" s="29" t="s">
         <v>5</v>
       </c>
-      <c r="O5" s="25"/>
-      <c r="P5" s="25"/>
-      <c r="Q5" s="25"/>
-      <c r="R5" s="25" t="s">
+      <c r="O5" s="29"/>
+      <c r="P5" s="29"/>
+      <c r="Q5" s="29"/>
+      <c r="R5" s="29" t="s">
         <v>6</v>
       </c>
-      <c r="S5" s="25"/>
-      <c r="T5" s="25"/>
-      <c r="U5" s="25"/>
-      <c r="V5" s="25" t="s">
+      <c r="S5" s="29"/>
+      <c r="T5" s="29"/>
+      <c r="U5" s="29"/>
+      <c r="V5" s="29" t="s">
         <v>7</v>
       </c>
-      <c r="W5" s="25"/>
-      <c r="X5" s="25"/>
-      <c r="Y5" s="25"/>
-      <c r="Z5" s="25"/>
-      <c r="AA5" s="25" t="s">
+      <c r="W5" s="29"/>
+      <c r="X5" s="29"/>
+      <c r="Y5" s="29"/>
+      <c r="Z5" s="29"/>
+      <c r="AA5" s="29" t="s">
         <v>8</v>
       </c>
-      <c r="AB5" s="25"/>
-      <c r="AC5" s="25"/>
-      <c r="AD5" s="25"/>
-      <c r="AE5" s="25" t="s">
+      <c r="AB5" s="29"/>
+      <c r="AC5" s="29"/>
+      <c r="AD5" s="29"/>
+      <c r="AE5" s="29" t="s">
         <v>9</v>
       </c>
-      <c r="AF5" s="25"/>
-      <c r="AG5" s="25"/>
-      <c r="AH5" s="25"/>
-      <c r="AI5" s="25" t="s">
+      <c r="AF5" s="29"/>
+      <c r="AG5" s="29"/>
+      <c r="AH5" s="29"/>
+      <c r="AI5" s="29" t="s">
         <v>10</v>
       </c>
-      <c r="AJ5" s="25"/>
-      <c r="AK5" s="25"/>
-      <c r="AL5" s="25"/>
-      <c r="AM5" s="25" t="s">
+      <c r="AJ5" s="29"/>
+      <c r="AK5" s="29"/>
+      <c r="AL5" s="29"/>
+      <c r="AM5" s="29" t="s">
         <v>11</v>
       </c>
-      <c r="AN5" s="25"/>
-      <c r="AO5" s="25"/>
-      <c r="AP5" s="25"/>
-      <c r="AQ5" s="25"/>
+      <c r="AN5" s="29"/>
+      <c r="AO5" s="29"/>
+      <c r="AP5" s="29"/>
+      <c r="AQ5" s="29"/>
     </row>
     <row r="6" spans="1:56" s="8" customFormat="1" x14ac:dyDescent="0.3">
       <c r="A6" s="4"/>
@@ -1330,9 +1329,9 @@
       <c r="D10" s="15"/>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
-      <c r="G10" s="32"/>
-      <c r="H10" s="32"/>
-      <c r="I10" s="32"/>
+      <c r="G10" s="25"/>
+      <c r="H10" s="25"/>
+      <c r="I10" s="25"/>
       <c r="J10" s="14"/>
       <c r="K10" s="14"/>
       <c r="L10" s="14"/>
@@ -1379,9 +1378,9 @@
       <c r="E11" s="14"/>
       <c r="F11" s="14"/>
       <c r="G11" s="14"/>
-      <c r="H11" s="33"/>
-      <c r="I11" s="33"/>
-      <c r="J11" s="33"/>
+      <c r="H11" s="26"/>
+      <c r="I11" s="26"/>
+      <c r="J11" s="26"/>
       <c r="K11" s="14"/>
       <c r="L11" s="14"/>
       <c r="M11" s="14"/>
@@ -1430,11 +1429,11 @@
       <c r="H12" s="14"/>
       <c r="I12" s="14"/>
       <c r="J12" s="14"/>
-      <c r="K12" s="34"/>
-      <c r="L12" s="34"/>
-      <c r="M12" s="34"/>
-      <c r="N12" s="34"/>
-      <c r="O12" s="34"/>
+      <c r="K12" s="27"/>
+      <c r="L12" s="27"/>
+      <c r="M12" s="27"/>
+      <c r="N12" s="27"/>
+      <c r="O12" s="27"/>
       <c r="P12" s="14"/>
       <c r="Q12" s="14"/>
       <c r="R12" s="14"/>
@@ -1843,17 +1842,17 @@
       <c r="AQ20" s="14"/>
     </row>
     <row r="21" spans="2:43" x14ac:dyDescent="0.3">
-      <c r="B21" s="35" t="s">
+      <c r="B21" s="14" t="s">
         <v>50</v>
       </c>
       <c r="C21" s="23">
         <v>45200</v>
       </c>
       <c r="D21" s="14"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="33"/>
-      <c r="G21" s="33"/>
-      <c r="H21" s="33"/>
+      <c r="E21" s="26"/>
+      <c r="F21" s="26"/>
+      <c r="G21" s="26"/>
+      <c r="H21" s="26"/>
       <c r="I21" s="14"/>
       <c r="J21" s="14"/>
       <c r="K21" s="14"/>
@@ -1895,20 +1894,20 @@
         <v>28</v>
       </c>
       <c r="C22" s="23">
-        <v>45209</v>
+        <v>45240</v>
       </c>
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
       <c r="F22" s="14"/>
-      <c r="G22" s="34"/>
-      <c r="H22" s="34"/>
-      <c r="I22" s="34"/>
-      <c r="J22" s="34"/>
-      <c r="K22" s="34"/>
-      <c r="L22" s="34"/>
-      <c r="M22" s="34"/>
-      <c r="N22" s="34"/>
-      <c r="O22" s="34"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="27"/>
+      <c r="K22" s="27"/>
+      <c r="L22" s="27"/>
+      <c r="M22" s="27"/>
+      <c r="N22" s="27"/>
+      <c r="O22" s="27"/>
       <c r="P22" s="14"/>
       <c r="Q22" s="14"/>
       <c r="R22" s="14"/>
@@ -1948,15 +1947,15 @@
       <c r="D23" s="14"/>
       <c r="E23" s="14"/>
       <c r="F23" s="14"/>
-      <c r="G23" s="36"/>
-      <c r="H23" s="36"/>
-      <c r="I23" s="36"/>
-      <c r="J23" s="36"/>
-      <c r="K23" s="36"/>
-      <c r="L23" s="36"/>
-      <c r="M23" s="36"/>
-      <c r="N23" s="36"/>
-      <c r="O23" s="36"/>
+      <c r="G23" s="28"/>
+      <c r="H23" s="28"/>
+      <c r="I23" s="28"/>
+      <c r="J23" s="28"/>
+      <c r="K23" s="28"/>
+      <c r="L23" s="28"/>
+      <c r="M23" s="28"/>
+      <c r="N23" s="28"/>
+      <c r="O23" s="28"/>
       <c r="P23" s="14"/>
       <c r="Q23" s="14"/>
       <c r="R23" s="14"/>
@@ -1996,15 +1995,15 @@
       <c r="D24" s="14"/>
       <c r="E24" s="14"/>
       <c r="F24" s="14"/>
-      <c r="G24" s="36"/>
-      <c r="H24" s="36"/>
-      <c r="I24" s="36"/>
-      <c r="J24" s="36"/>
-      <c r="K24" s="36"/>
-      <c r="L24" s="36"/>
-      <c r="M24" s="36"/>
-      <c r="N24" s="36"/>
-      <c r="O24" s="36"/>
+      <c r="G24" s="28"/>
+      <c r="H24" s="28"/>
+      <c r="I24" s="28"/>
+      <c r="J24" s="28"/>
+      <c r="K24" s="28"/>
+      <c r="L24" s="28"/>
+      <c r="M24" s="28"/>
+      <c r="N24" s="28"/>
+      <c r="O24" s="28"/>
       <c r="P24" s="14"/>
       <c r="Q24" s="14"/>
       <c r="R24" s="14"/>
@@ -2092,15 +2091,15 @@
       <c r="D26" s="14"/>
       <c r="E26" s="14"/>
       <c r="F26" s="14"/>
-      <c r="G26" s="36"/>
-      <c r="H26" s="36"/>
-      <c r="I26" s="36"/>
-      <c r="J26" s="36"/>
-      <c r="K26" s="36"/>
-      <c r="L26" s="36"/>
-      <c r="M26" s="36"/>
-      <c r="N26" s="36"/>
-      <c r="O26" s="36"/>
+      <c r="G26" s="28"/>
+      <c r="H26" s="28"/>
+      <c r="I26" s="28"/>
+      <c r="J26" s="28"/>
+      <c r="K26" s="28"/>
+      <c r="L26" s="28"/>
+      <c r="M26" s="28"/>
+      <c r="N26" s="28"/>
+      <c r="O26" s="28"/>
       <c r="P26" s="14"/>
       <c r="Q26" s="14"/>
       <c r="R26" s="14"/>

</xml_diff>